<commit_message>
Added validation for relationships
</commit_message>
<xml_diff>
--- a/test-artifacts/media-reports/broken-media.xlsx
+++ b/test-artifacts/media-reports/broken-media.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -421,90 +421,315 @@
       <c r="F1" t="str">
         <v>status</v>
       </c>
+      <c r="G1" t="str">
+        <v>ok</v>
+      </c>
+      <c r="H1" t="str">
+        <v>error</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>3-2</v>
+        <v>B2-W1</v>
       </c>
       <c r="B2" t="str">
-        <v>http://drupal-geneseo-backup.ddev.site/basic_page/journals-and-reflections/</v>
+        <v>http://localhost/sunny/accessibility-office/documentation-criteria</v>
       </c>
       <c r="C2" t="str">
-        <v>http://drupal-geneseo-backup.ddev.site/sites/default/files/sites/404%20Page/page-not-found-graphic.jpg</v>
+        <v>http://localhost/sunny/sites/default/files/sites/dean_office/Acquired%20Brain%20Injury%20Documentation%20Form%20SUNY%20Geneseo.pdf</v>
       </c>
       <c r="D2" t="str">
-        <v>image</v>
+        <v>pdf</v>
       </c>
       <c r="E2" t="str">
-        <v>/sites/default/files/sites/404%20Page/page-not-found-graphic.jpg</v>
+        <v>http://localhost/sunny/sites/default/files/sites/dean_office/Acquired%20Brain%20Injury%20Documentation%20Form%20SUNY%20Geneseo.pdf</v>
       </c>
       <c r="F2">
         <v>404</v>
+      </c>
+      <c r="G2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>3-1</v>
+        <v>B2-W1</v>
       </c>
       <c r="B3" t="str">
-        <v>http://drupal-geneseo-backup.ddev.site/basic_page/boiling-flasks-round-bottom/</v>
+        <v>http://localhost/sunny/accessibility-office/documentation-criteria</v>
       </c>
       <c r="C3" t="str">
-        <v>http://drupal-geneseo-backup.ddev.site/sites/default/files/sites/404%20Page/page-not-found-graphic.jpg</v>
+        <v>http://localhost/sunny/sites/default/files/sites/dean_office/Attention%20Deficit%20Documentation.pdf</v>
       </c>
       <c r="D3" t="str">
-        <v>image</v>
+        <v>pdf</v>
       </c>
       <c r="E3" t="str">
-        <v>/sites/default/files/sites/404%20Page/page-not-found-graphic.jpg</v>
+        <v>http://localhost/sunny/sites/default/files/sites/dean_office/Attention%20Deficit%20Documentation.pdf</v>
       </c>
       <c r="F3">
         <v>404</v>
+      </c>
+      <c r="G3" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>3-2</v>
+        <v>B2-W1</v>
       </c>
       <c r="B4" t="str">
-        <v>http://drupal-geneseo-backup.ddev.site/basic_page/conh35clcl2-prep/</v>
+        <v>http://localhost/sunny/accessibility-office/documentation-criteria</v>
       </c>
       <c r="C4" t="str">
-        <v>http://drupal-geneseo-backup.ddev.site/sites/default/files/sites/404%20Page/page-not-found-graphic.jpg</v>
+        <v>http://localhost/sunny/sites/default/files/sites/dean_office/Autism%20Spectrum%20Documentation%20Form.pdf</v>
       </c>
       <c r="D4" t="str">
-        <v>image</v>
+        <v>pdf</v>
       </c>
       <c r="E4" t="str">
-        <v>/sites/default/files/sites/404%20Page/page-not-found-graphic.jpg</v>
+        <v>http://localhost/sunny/sites/default/files/sites/dean_office/Autism%20Spectrum%20Documentation%20Form.pdf</v>
       </c>
       <c r="F4">
         <v>404</v>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>3-1</v>
+        <v>B2-W1</v>
       </c>
       <c r="B5" t="str">
-        <v>http://drupal-geneseo-backup.ddev.site/basic_page/mofs-part-3/</v>
+        <v>http://localhost/sunny/accessibility-office/documentation-criteria</v>
       </c>
       <c r="C5" t="str">
-        <v>http://drupal-geneseo-backup.ddev.site/sites/default/files/sites/404%20Page/page-not-found-graphic.jpg</v>
+        <v>http://localhost/sunny/sites/default/files/sites/dean_office/Deaf%20and%20HH%20documentation.pdf</v>
       </c>
       <c r="D5" t="str">
-        <v>image</v>
+        <v>pdf</v>
       </c>
       <c r="E5" t="str">
-        <v>/sites/default/files/sites/404%20Page/page-not-found-graphic.jpg</v>
+        <v>http://localhost/sunny/sites/default/files/sites/dean_office/Deaf%20and%20HH%20documentation.pdf</v>
       </c>
       <c r="F5">
         <v>404</v>
+      </c>
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>B2-W1</v>
+      </c>
+      <c r="B6" t="str">
+        <v>http://localhost/sunny/accessibility-office/documentation-criteria</v>
+      </c>
+      <c r="C6" t="str">
+        <v>http://localhost/sunny/sites/default/files/sites/dean_office/Learning%20Disabilities%20Documentation%20Guidelines.pdf</v>
+      </c>
+      <c r="D6" t="str">
+        <v>pdf</v>
+      </c>
+      <c r="E6" t="str">
+        <v>http://localhost/sunny/sites/default/files/sites/dean_office/Learning%20Disabilities%20Documentation%20Guidelines.pdf</v>
+      </c>
+      <c r="F6">
+        <v>404</v>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>B2-W1</v>
+      </c>
+      <c r="B7" t="str">
+        <v>http://localhost/sunny/accessibility-office/documentation-criteria</v>
+      </c>
+      <c r="C7" t="str">
+        <v>http://localhost/sunny/sites/default/files/sites/dean_office/Chronic%20Health%20Conditions%20Documentation.pdf</v>
+      </c>
+      <c r="D7" t="str">
+        <v>pdf</v>
+      </c>
+      <c r="E7" t="str">
+        <v>http://localhost/sunny/sites/default/files/sites/dean_office/Chronic%20Health%20Conditions%20Documentation.pdf</v>
+      </c>
+      <c r="F7">
+        <v>404</v>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>B2-W1</v>
+      </c>
+      <c r="B8" t="str">
+        <v>http://localhost/sunny/accessibility-office/documentation-criteria</v>
+      </c>
+      <c r="C8" t="str">
+        <v>http://localhost/sunny/sites/default/files/sites/dean_office/CONCUSSION%20EVALUATION.pdf</v>
+      </c>
+      <c r="D8" t="str">
+        <v>pdf</v>
+      </c>
+      <c r="E8" t="str">
+        <v>http://localhost/sunny/sites/default/files/sites/dean_office/CONCUSSION%20EVALUATION.pdf</v>
+      </c>
+      <c r="F8">
+        <v>404</v>
+      </c>
+      <c r="G8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>B2-W1</v>
+      </c>
+      <c r="B9" t="str">
+        <v>http://localhost/sunny/accessibility-office/documentation-criteria</v>
+      </c>
+      <c r="C9" t="str">
+        <v>http://localhost/sunny/sites/default/files/sites/dean_office/Mobility%20Impairment%20Documentation.pdf</v>
+      </c>
+      <c r="D9" t="str">
+        <v>pdf</v>
+      </c>
+      <c r="E9" t="str">
+        <v>http://localhost/sunny/sites/default/files/sites/dean_office/Mobility%20Impairment%20Documentation.pdf</v>
+      </c>
+      <c r="F9">
+        <v>404</v>
+      </c>
+      <c r="G9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>B2-W1</v>
+      </c>
+      <c r="B10" t="str">
+        <v>http://localhost/sunny/accessibility-office/documentation-criteria</v>
+      </c>
+      <c r="C10" t="str">
+        <v>http://localhost/sunny/sites/default/files/sites/dean_office/Neurological%20Disorders%20Documentation.pdf</v>
+      </c>
+      <c r="D10" t="str">
+        <v>pdf</v>
+      </c>
+      <c r="E10" t="str">
+        <v>http://localhost/sunny/sites/default/files/sites/dean_office/Neurological%20Disorders%20Documentation.pdf</v>
+      </c>
+      <c r="F10">
+        <v>404</v>
+      </c>
+      <c r="G10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>B2-W1</v>
+      </c>
+      <c r="B11" t="str">
+        <v>http://localhost/sunny/accessibility-office/documentation-criteria</v>
+      </c>
+      <c r="C11" t="str">
+        <v>http://localhost/sunny/sites/default/files/sites/dean_office/Psychological%20Conditions%20Documentation.pdf</v>
+      </c>
+      <c r="D11" t="str">
+        <v>pdf</v>
+      </c>
+      <c r="E11" t="str">
+        <v>http://localhost/sunny/sites/default/files/sites/dean_office/Psychological%20Conditions%20Documentation.pdf</v>
+      </c>
+      <c r="F11">
+        <v>404</v>
+      </c>
+      <c r="G11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>B2-W1</v>
+      </c>
+      <c r="B12" t="str">
+        <v>http://localhost/sunny/accessibility-office/documentation-criteria</v>
+      </c>
+      <c r="C12" t="str">
+        <v>http://localhost/sunny/sites/default/files/sites/dean_office/Temporary%20Impairments%20Documentation.pdf</v>
+      </c>
+      <c r="D12" t="str">
+        <v>pdf</v>
+      </c>
+      <c r="E12" t="str">
+        <v>http://localhost/sunny/sites/default/files/sites/dean_office/Temporary%20Impairments%20Documentation.pdf</v>
+      </c>
+      <c r="F12">
+        <v>404</v>
+      </c>
+      <c r="G12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>B2-W1</v>
+      </c>
+      <c r="B13" t="str">
+        <v>http://localhost/sunny/accessibility-office/documentation-criteria</v>
+      </c>
+      <c r="C13" t="str">
+        <v>http://localhost/sunny/sites/default/files/sites/dean_office/Visual%20Impairment%20Documentation.pdf</v>
+      </c>
+      <c r="D13" t="str">
+        <v>pdf</v>
+      </c>
+      <c r="E13" t="str">
+        <v>http://localhost/sunny/sites/default/files/sites/dean_office/Visual%20Impairment%20Documentation.pdf</v>
+      </c>
+      <c r="F13">
+        <v>404</v>
+      </c>
+      <c r="G13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>B1-W2</v>
+      </c>
+      <c r="B14" t="str">
+        <v>http://localhost/sunny/aac/forms-and-documents</v>
+      </c>
+      <c r="C14" t="str">
+        <v>http://localhost/sites/default/files/users/1120/Continuing%20Recognition%20Form.pdf</v>
+      </c>
+      <c r="D14" t="str">
+        <v>pdf</v>
+      </c>
+      <c r="E14" t="str">
+        <v>http://localhost/sites/default/files/users/1120/Continuing%20Recognition%20Form.pdf</v>
+      </c>
+      <c r="F14">
+        <v>404</v>
+      </c>
+      <c r="G14" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H14"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>